<commit_message>
Get daily reddit data: Tue Apr 23 08:08:24 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_28.xlsx
+++ b/data/2024_04_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C465"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2794 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1cayos6</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Fun nails</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cayos6</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1caxesz</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Unhappy with manicure?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1caxesz/unhappy_with_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1cawqkq</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>15% discount on press on nails</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/promotion/psp/A1BYNCS4NHPZ55</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1cawj2w</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>practicing nail art designs!</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2sx19eux5wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1cass3r</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to paint my nails properly </t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cass3r/how_to_paint_my_nails_properly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1carcts</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Nail tech having retention issues</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1carcts/nail_tech_having_retention_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1capt1l</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>week nails</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1capt1l/week_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1cavfaa</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>I don't have long nails but I want to shout out my nail technician for making my nails look amazing everytime.</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cavfaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1caualr</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Shoes for nail tech</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1caualr/shoes_for_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1catvsp</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>what do you think? I've had my 3D nails, autumn color for 14 days 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1catvsp</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1catv1x</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>How it started vs. how it’s going</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1catv1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1catd8z</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1catd8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1catc6p</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Lilac</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2433y0k35wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1cat5q4</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Might be dumb question but</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cat5q4/might_be_dumb_question_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1caspnn</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>I’m getting faster!!!</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plr211kby4wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1cas3pi</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Pretty little butterfly 💙</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cas3pi</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1carg4u</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>I have a formal event and i'm lost every bit of the way with my hands</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1carg4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1car6r6</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Obsessed with this new set</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x426robel4wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1car58k</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sunset nails 🌅 </t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3v1mayp1l4wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1car1a8</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>freestyle nails 💅🏽⭐️</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1car1a8</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1caqs34</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Blue aura 🧿</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xt4mlsl0i4wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1caqkyu</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Obsessed with my new nails 🩷</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utjz6zgcg4wc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1capthm</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Elopement/Grad Nails</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1capthm</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1capr8p</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Can’t stop staring at them</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dsw0uhxj94wc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1capp09</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Red Bottoms</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1capp09</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1capkzr</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>nails I made for my stepdaughter ✨</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pxjyz1a84wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1capgnl</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>plain jane</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15ov14yb74wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1capdfe</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Esthetician with a nail question </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1capdfe/esthetician_with_a_nail_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1caoxl2</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Doing a bridal set after so long(set done by me)</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwkxg1z834wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1caojc2</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Does this mani wash me out?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caojc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1cam8s7</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cam8s7</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1cam2zg</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>tips pls</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cam2zg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1caf20v</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>need advice on nail salon cleanliness</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/405nzun342wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1caoj12</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Is navy nails for a navy dress too much?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1caoj12/is_navy_nails_for_a_navy_dress_too_much/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1caekbu</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Clubbed thumbs :( I have (and hate!) them. Is this the best nail shape for me? I’ve never had them so long and worry they might look stupid.</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caekbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1caeav3</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>hey all! absolute beginner here looking for help building a kit from zero!</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1caeav3/hey_all_absolute_beginner_here_looking_for_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1cao66l</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>My nails after 3 months</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cao66l</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1canxsy</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>My first time with gel-x + 3 weeks!</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1canxsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1cand6a</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Spring has sprung 🌸</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgayh901s3wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1can484</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Got my nails done at “Luke’s nails and spa in somerdale nj” thoughts?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqmkfaxaq3wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1cam6bn</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do u think of this goth set? I really love it. It's perfect for my birthday </t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xlhhvxxj3wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1cam2u2</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Checker Nails</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cam2u2</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1calsxp</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Loving jelly nails!!!</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhuagdtmh3wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1calnbl</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Using Foils</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1calnbl/using_foils/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1cal12u</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Happy Passover to those who celebrate!</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n12sjrav93wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1cakv7b</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>These would be perfect wedding nails!</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cakv7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1cakaf4</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>My favorite DIY manicure yet</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cakaf4</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1cak95o</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>New nails. What do you think?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43celptg43wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1cajr06</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>How do I commit to keeping my nails nice?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cajr06</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1cajid9</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>A little girl said I had fairy nails😌</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cajid9</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1caj8u1</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Nails for my birthday!</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caj8u1</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1caiqt0</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Obsessed with my nails for my sister's wedding!!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrmhi4f1u2wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1caicpu</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>My new yellow girls</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8annqtr9r2wc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1caiaez</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love doing my nails in a new model with shiny ones. </t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vo54yhavq2wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1cahiyn</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>I had this nailart done on my hands twice, it's just so delicate and beatiful 💖🥰</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7wfsbfll2wc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1cah8b6</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Waiting for Summer 💕</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnb74nbij2wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1cah0yo</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Hand sculpted Patrick &amp; Gary Sponge bob nails 🫧🪼 look at the little jelly fishes 🥹🩷🪼</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cah0yo</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1cagwec</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Nail recs for this dress?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cagwec/nail_recs_for_this_dress/</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1cagh5p</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Update from the horrible manicure I got yesterday..</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cagh5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1cafwqg</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>2 years of progress 😌😌</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cafwqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1caf54w</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>trouble removing dip</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4e3t9x1q42wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1caf2rr</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ombre press on nails </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyawfv3942wc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1caeyp3</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>New nails im loving</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caeyp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1caeq38</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>favorite set I’ve ever had!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/biciag1q12wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1caed0k</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>OH NO I JUST NOTICED MY NAIL BROKE IN MY SLEEP</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caed0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1cae0nt</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>When the absolutely fuckkkkk did A BASIC GEL Manicure cost 100 !!! Nothing crazy either short set</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cae0nt/when_the_absolutely_fuckkkkk_did_a_basic_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1cac8i9</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Can anyone recommend a non-UV pastel holographic nail polish?</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cac8i9/can_anyone_recommend_a_nonuv_pastel_holographic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1ca8mdg</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>The blue is back💙🦋🥶</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ca8mdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1cadoy9</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Can I get a fill after only 11 days?</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gugz7v57u1wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1c9ycb0</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>One month progress</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftrjladknxvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1cadgot</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>My wedding nails 👰‍♀️</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wz27dg1ks1wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1c9vz6p</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>How did I not know brush on nail glue existed!! I’ve been struggling with the tiny little tube whenever I do my nails. The game has been changed omg</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5x9g3q2r2xvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1c9tm6d</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Damaged nails after SNS + what to do instead</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c9tm6d/damaged_nails_after_sns_what_to_do_instead/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1c9oahj</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>so so happy w these</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0id3je10hvvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1cachs1</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Whaddya think?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dnxa04ol1wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1cacaa5</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Spring French Nails</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddiwp4j3k1wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1cabk7v</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Tips Pls - Nail Journey</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cabk7v/tips_pls_nail_journey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1ca9wdb</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Does anyone else make their own press ons with gel tips?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ca9wdb/does_anyone_else_make_their_own_press_ons_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1ca9r5y</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>After 24 years of nail biting I got into doing my nails with gel. My nails have never been this long 😭 attempt 1 - 4</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ca9r5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1ca9aec</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried doing marble nails by myself! </t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cseuyqmuw0wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1ca8tpc</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>chose classic red for this week 🌹</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9feht04vs0wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1ca8oi7</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Top Coat for Dip Powder</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ca8oi7/top_coat_for_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1ca7ajy</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>did these for fun</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62jvw7nsc0wc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1ca73eq</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Which shape looks better?</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/do9132nha0wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1ca6zr4</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Better Sunken Secrets pic </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqpsq30a90wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1ca5e8c</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>One of my faves 💙</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nqf56alpzvc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1ca5c1f</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>How to avoid that thing where you skin comes off near your nails.</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ca5c1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1cay71x</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the shiftiest shift to have ever shifted in the history of shifts </t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/adb945aah6wc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1cawsqw</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Kbshimmer recs?</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cawsqw/kbshimmer_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1cawagm</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Selene by Phoenix Indie</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmq8aymcv5wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1cavhn1</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>How do I stop ruining my nail art with topcoat??</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptmqxpu7n5wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1cavczc</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>trouble removing dip</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dv84b7twl5wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1cattja</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>FIRST coat of ilnp pink suede with 10lb magnet (over mooncat getting even base)</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vytw1pqt75wc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1catf6k</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Are these flakies too much or just right?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1catf6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1casfgd</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Clouds on chrome</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hsnwwpvv4wc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1carutq</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>ILNP Love: Fairy Dust &amp; Pool Party</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76rjqa20r4wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1car6gb</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Harper by ILNP in motion </t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uzddg9pbl4wc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1carabo</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Strawberry season!</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1carabo</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1caqg0e</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Orange cat 🐈 vibes today 🧡</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caqg0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1caq299</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Mooncat Fake Halo</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caq299</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1capyka</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>First try at nail wraps</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1capyka</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1capoa5</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>I found the perfect nude jelly for me</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/st99dwrz84wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1cap2fu</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Distorted Checker Nails</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cap2fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1caoyr2</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>For Earth Day - Jeff’s Inn By The Sea aka the shimmeriest green that ever shimmered green.</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caoyr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1caojab</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Velvet Rose Magnetic Tips</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caojab</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1caogx5</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Omg Y'all 😂</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caogx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1cao4mx</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Wizard duel by Starrily</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cao4mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1can4kt</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Dark Omens and glitter</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1can4kt</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1ca62fh</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>What can I do to make them look good?</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/by68wxr2yzvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1ca8lz2</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When are Zoya discounts happening </t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ca8lz2/when_are_zoya_discounts_happening/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1camn88</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Cock-a-Doodle-DOOM 💜❤️‍🔥 in celebration of getting my baby chicks</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1camn88</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1camctn</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>A Wee Bit of Dazzle Dry Love</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1camctn/a_wee_bit_of_dazzle_dry_love/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1calwo1</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Boolba redux</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1calwo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1caltd9</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Polished For Days, Blossom 🧡🌸🍑🌷🌅🩷</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfedui7ph3wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1cafc3y</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Needing advice/yips</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qlbmchk362wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1cal3h3</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>obsessed with how shiny my dragon scales are</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cal3h3</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1cajvyw</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Coronation ‘24 for today</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cajvyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1cajrmo</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Minty holo goodness ❇️</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81swsu6113wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1cajplx</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Trying out yellow 💛</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cajplx</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1cajerg</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>“no polish” polish 🫧</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ayx4uy0oy2wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1caj9n2</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Treachery in the Blue</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caj9n2</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1caj6kb</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Nailtiques Formula 2 - great news!</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1caj6kb/nailtiques_formula_2_great_news/</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1cai6qi</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Catch my drift</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cai6qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1cahvru</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Try not to panic 😭😭😭</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/112sa9m0o2wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1caht30</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>For the brown &amp; gold 💛</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caht30</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1cahl6n</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Boolba...</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cahl6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1cagjlg</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Nude</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlhcfsple2wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1cafzrf</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Gel CleanUp Help</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cafzrf/gel_cleanup_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1cafp2k</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Too much work</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cafp2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1cafk2c</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>What to do when nail polish just won’t come off?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cafk2c/what_to_do_when_nail_polish_just_wont_come_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1caffh2</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Polished for Days Lush is SO Shifty</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caffh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1caex5b</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Mobius from Cirque is actually unreal</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wze1fc2532wc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1caer8n</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Obsessed with iridescents right now</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkzz0z6y12wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1caecuh</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>How do you use sheers?</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1caecuh/how_do_you_use_sheers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1cae8fx</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Till death do us part</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cae8fx</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1cadprb</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Picture Curable after one week of wear</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cadprb</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1caclig</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UK gang horseshoe magnet update </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8q1z7g0em1wc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1cac2uy</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>🏅💙Favorite Cerulean💙🏅</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cac2uy</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1cabtzs</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Witchy nails? Or burnt nails? Either way I love it.</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cabtzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1caboyi</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Helter Seltzer is so underrated!</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caboyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1caabtt</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>It's Everything I Thought it Would Be - Sabertooth</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caabtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1ca9jum</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So thermals can be neutrals too...who knew? </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0b1o6h95z0wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1ca9jeg</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>So shimmery</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ca9jeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1ca9ior</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Gumdrop Mountains</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ca9ior</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1ca9hnh</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>My favorite purple multichrome 💜</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ca9hnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1ca87kw</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Hopped on the Cock a Doodle Doom Train 💜🧡</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/PZthajZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1ca6xps</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nothing says therapy is working like picking up old passions - I lost my motivation for nail art/self care for the past few years, but have really enjoyed exploring it again with some spring flowers 🌺 </t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g92el9cm80wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1ca6vvu</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ca6vvu/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1ca5zrq</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Second panned polish!!</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ca5zrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1ca5emq</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>One of my faves!</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2xpgvtqpzvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1caxfoa</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Working on my own set! </t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ro9tivh886wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1cawkum</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Perfect Beach Trip Nails</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rh2dnmbdy5wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1cau4fd</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>earth day nails :p</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cau4fd</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1catec5</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>When your man is you practice sheet</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tto9x7c345wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1caqyjq</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>i felt like doing a dramatic set 🤍🩷</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caqyjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1captc0</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Red Bottoms</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1captc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1cap2tx</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>fingernail on a fingernail</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yti2nrqc44wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1caox7n</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>My official comeback</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqjzh9x634wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1cah8sd</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Waiting for Summer 💕</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dm64kdulj2wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1cah1mn</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Hand sculpted Patrick &amp; Gary Sponge bob nails 🫧🪼 look at the little jelly fishes 🥹🩷🪼</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cah1mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1cabf0k</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Just a little bling.</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cabf0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1ca9ip2</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>I painted scream nails. How do they look?</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wxt4y46vy0wc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1ca9b33</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Butterfly Nails</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfkcqo32x0wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1ca6okf</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Got inspired by the irises in my mom's garden 🤗🤗</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ca6okf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Apr 24 08:09:21 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_28.xlsx
+++ b/data/2024_04_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C465"/>
+  <dimension ref="A1:C615"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8338,6 +8338,2556 @@
         </is>
       </c>
     </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1cbsgt2</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Favorite set I ever had done 🤍</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mb2ol9gtdwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1cbsggp</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>My latest set 🩵🩵🩵</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8mpoaobtdwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1cbrkbo</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>henna nails</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bggwiha4idwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1cbqtah</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>using apres gelx tips to do press ons?</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cbqtah/using_apres_gelx_tips_to_do_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1cbpw8j</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>These took FOREVER</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbpw8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1cborz7</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cborz7/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1cbnifv</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>newest set 😍🤍 by @nails.by.carla_ on IG!</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/154403t4ccwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1cbmc4v</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Ghibli Inspired 💕🐉🪄👒</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbmc4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1cbhfw1</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/igc314a3yawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1cbp33j</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>i’m going crazy over this floral set i made the other day 😩😩😩 i never want to take them off!!!</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbp33j</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1cbetsc</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>My gel nails keeps coming off</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cbetsc/my_gel_nails_keeps_coming_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1cbcgpr</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>This weeks mani 💙💜</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbcgpr</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1cbat4a</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t xml:space="preserve">any tips are appreciated </t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2ju5uq4n9wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1cboqhf</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Orange Nails?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cboqhf</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1cbo3yb</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Did my own toes! How did I do?</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbo3yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1cbnhfc</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painting a Billie eilish press on set 🥑 iconic green version first </t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5zplicovbcwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1cbmf1k</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Cat eye checkerboard!</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85b857qk2cwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1cbl888</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Cat Eye Nails</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dle7lyoasbwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1cbkyx4</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new set from a place ive never been! love them 🎀 </t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkxpy8d1qbwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1cbkual</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Impressed by Impress Nails</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbkual</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1cbkgag</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>In my Aura Era ✨</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0bpfymtmlbwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1cbk80j</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Pop of blue</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dthrfknjbwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1cbk7fl</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newly Trim And Yellow For Spring!           </t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cbk7fl/newly_trim_and_yellow_for_spring/</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1cbjy86</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to find a good bridal color for nails with ridges so it can’t be sheer. This is a little too pink any recommendations? </t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ttiwihxghbwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1cbjrzu</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>the worst my nails have ever been</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gasqrp33gbwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1cbjcq2</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Something different; love or hate?!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbjcq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1cbiv15</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>love my first gel x mani but…</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/osqki61q8bwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1cbiuur</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>My nail tech is my lifeline.</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7p6czko8bwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1cbimvr</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Team 🍒 or 🍓?</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbimvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1cbi08v</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>wine nails💘</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8o89t8da2bwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1cbhslo</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Should nail techs reuse toe separators?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cbhslo/should_nail_techs_reuse_toe_separators/</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1cbh86x</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Transfemme new to nails how do these look</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7jlisslwawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1cbh2jt</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>What is the cause of this?</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8z5nivgvawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1cbgz60</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Trying out nail charms</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbgz60</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1cbgwzr</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Im in love with my set from today</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/955z2l5cuawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1cbgv8e</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ie1cht30uawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1cbgnfb</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>my hawaii nails</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/slw7ja4gsawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1cbger9</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>What is the difference?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbger9</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1cbgdkk</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Would you automatically clock these as press-ons?</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhoztthjqawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1cbfbyj</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>As an ex-chronic nail biter, i have all the rights to flex. 🥰</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bbpzki5jawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1cbf63d</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matte black nail polish? </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cbf63d/matte_black_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1cbezs1</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Cyclone</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbezs1</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1cbevzn</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>New to the Game</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cbevzn/new_to_the_game/</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1cbekkk</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Manicure set recommendations (possibly in Germany)</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cbekkk/manicure_set_recommendations_possibly_in_germany/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1cbe6iu</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Nail tips??</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbe6iu</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1cbdsdn</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Black floral</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q4hhawl28awc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1cbdqld</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>This blue🥹💎</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvcl36wx7awc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1cbdmjz</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Ridges in nails</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cbdmjz/ridges_in_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1cbdaaw</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails!!!! </t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0wjmgrp4awc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1cbc8k0</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Summer please?</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbc8k0</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1cbc7ue</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Making summer nails but it won’t stop raining😢</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbc7ue</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1cbc18i</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>New nail place!</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbc18i</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1cbbusn</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Can it be saved?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nu45hreiu9wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1cbb7dh</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Soft Nails</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkcz3ebxp9wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1cbaplk</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Nail Salon Memberships</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cbaplk/nail_salon_memberships/</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1cbakvf</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Soft pink set</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbakvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1cbak5q</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Loving these😍😍</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbak5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1cba94m</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Nail hardening polish recommendations</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cba94m/nail_hardening_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1cba8xv</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Loving the neon 😌</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cba8xv</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1cb9sao</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>glass peach with sparkle tip✨</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb9sao</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1cb9s0j</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Ocean Wave Nails</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fq71u7rf9wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1cb9psn</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Short but pretty, I don't know what this shade of green is called but I loved it.</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06t1tcmaf9wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1cb9iky</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Nail products (gel, acrylic, etc) never come off my nails??</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cb9iky/nail_products_gel_acrylic_etc_never_come_off_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1cb9iiq</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Some blobby work</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb9iiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1cb9ao1</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>New to nails! Question about acrylics….</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cb9ao1/new_to_nails_question_about_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1cb5hxg</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Manifesting spring with these nails</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ii2ce3fk8wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1caw25i</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Help! How do I fix a broken nail? 😭</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1caw25i</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1cb6h93</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>DIY Polygel Nails (Second Set)</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6buiffttr8wc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1cb6h7i</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>New pastel lilac nails with a twist</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb6h7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1cb69s8</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Russian Manicure with Coconut Milk Hard Gel Polish</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb69s8</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1cb686j</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Before and after is so satisfying</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb686j</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1cb5nbl</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>feeling spring-y 🌸</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb5nbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1cb549r</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Are these grown out enough for a fill?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb549r</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1cb3wve</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>My favorite nails</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdpndf2288wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1cb2wpn</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Is Dip powder more damaging than gel polish?</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cb2wpn/is_dip_powder_more_damaging_than_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1cb27yh</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Practice-nails</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb27yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1cb1cya</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Do you like this green?</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40ky37oxj7wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1cb0xai</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>This month’s cutie nails</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcn3edhye7wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1cb0l7s</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails </t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tch3hld2b7wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1cazzse</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>New nails by me on me</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cazzse</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1cbs68p</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>ORLY Color Pass Summer ‘24 - Cloudscape (swatches + comparisons + review)</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbs68p</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1cbrqty</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Had to match for 420!</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbrqty</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1cbrani</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>My Pet What?!</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbrani</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1cbpfse</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Stamps warm and cold</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbpfse</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1cboy4z</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Looking for a vintage Butter polish dupe</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cboy4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1cbomjb</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>What should I do about a lifting natural nail?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am58b15mmcwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1cbo4l3</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ISO: You Look Like You’ve Seen A Ghost by Bee’s Knees Lacquer </t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h9zi6athcwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1cbn72t</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>RV There Yet?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/okCupc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1cbn6su</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Cake Day Nails</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4e1t61289cwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1cbmdz2</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>For those who are familiar with Londontown concealers, which one might be best for olive skin?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cbmdz2/for_those_who_are_familiar_with_londontown/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1cbm6ev</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>I’m doing it, I’m reclaiming painted nails despite my abuse [potential TW]</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cbm6ev/im_doing_it_im_reclaiming_painted_nails_despite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1cbm1w5</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Help me find this color!</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbm1w5</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1cbler9</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Waiting for my Sally Beauty order to arrive like</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cbler9/waiting_for_my_sally_beauty_order_to_arrive_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1cbktco</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Peel off base and gel tips removal help</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymec7kfqobwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1cbkrol</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Dupe for DND DC 205 in regular polish?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbkrol</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1cbkizg</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>ILNP Fairy Dust Skittle</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbkizg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1cbkfgb</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Now what? </t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6uk585aflbwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1cbk7io</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Pre birthday manis #2 &amp; #3</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbk7io</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1cbj4v6</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Quicksand's Embrace is a really cute play on a neutral pink</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1y1rpa0x9bwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1cbivpj</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>ILNP Amber is stunning</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbivpj</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1cbis38</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Enchanting: Mooncat Millenium over a purple base (Sinful Colors "Let's Talk")</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9h7n9jx7bwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1cbingj</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>ILNP Velour Magnetized</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uy6mwpl57bwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1cbhrxs</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Traditional lacquer dupe request</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sb8e1l1k0bwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1cbhot4</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Bridesmaid nail recommendations</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbhot4</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1cbhna4</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>What it Takes 🧲</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8jaih8lzawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1cbgy3h</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Phoenix does no wrong in my eyes!</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8q67y90kuawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1cbgxdq</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>The Windy City by Dam Nail Polish</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e45eoeveuawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1cbgrvz</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Hello party people!!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbgrvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1cbgg20</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>"It's not a phase, mom!! 😒"</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jtk86yb0rawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1cbgeno</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Lost Berry (thermal) 💓</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbgeno</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1cbfvyc</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Picked out three polishes from Mooncat’s new Song of Sirens collection. This one is Am I Everything you Fear?.</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbfvyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1cbe71v</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Cuticle oil vs. Balm or cream?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cbe71v/cuticle_oil_vs_balm_or_cream/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1cbdtid</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Still feeling the blues this spring</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fti75yyh8awc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1cbde0o</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>This one really surprised me 🔥</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbde0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1cbamdu</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Suggestions</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4gxn5jql9wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1cbalrj</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Mooncat - Head in the Clouds</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbalrj</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1cbaioz</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>✨Tealing the Show✨</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cbaioz/tealing_the_show/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1cbaihy</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>How many sheer pinks do you own?? Me: yes</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbaihy</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1cbabtz</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Velvet magnetics have me in a chokehold</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gfzal5ykj9wc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1cb9sky</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Love these colors' interactions</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb9sky</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1cb9rt9</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Just when I'm convinced that I have enough polish...</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb9rt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1cb9fxz</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>What Dreams are Made of- Polished for Days</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bnru4ts9d9wc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1cb9bmc</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>My Portrait of an Introvert spontaneously exploded</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb9bmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1cb92hb</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Why does OPI Akoya Pearl dry bumpy?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb92hb</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1cb8qli</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Super happy with my first jelly!</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2b15gg389wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1cb7ym9</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>KL Polish (discontinued) - To The Stars</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6k6egtv29wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1cb7gay</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>🏅💙Favorite Blue💙🏅</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb7gay</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1cb5x6n</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>ILNP Pink Suede appreciation post</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb5x6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1cb5j2q</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>An update on the polish color I didn’t like: You all helped me troubleshoot and it has now lasted 9 days without a single chip (ILNP Clover)</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ug3ialknk8wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1cb4o2b</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Low-effort nail art 🖤</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7oxxii2e8wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1cb4mn4</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Moody Pansies with Holo Taco</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb4mn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1cb3x9p</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>“Groundbreaking…”</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb3x9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1cb3qg3</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Swatch request for other Trust the shimmer polishes from Dam</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pf489y9k68wc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1cb3dlh</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>LynB - Don't Go There</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb3dlh</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1cb2lp6</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Neon✨</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb2lp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1cb2ckk</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Picture Polish 💜 Be creative</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyuqyyw2u7wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1cb1jxk</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Long-lasting base + top coat combo - OPI/Essie/Sally Hansen</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cb1jxk/longlasting_base_top_coat_combo_opiessiesally/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1cb18ed</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Dupe for 20yo polish?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cb18ed</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1cbph81</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Thermal and stamps? Yes.</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbph81</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1cbott2</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Aura Nails!</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbott2</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1cbnmz7</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Distorted Checker Nails</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbnmz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1cbnav5</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painting a Billie eilish press on set 🥑 iconic green version first </t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vy5m6vd8acwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1cbkglk</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>In my Aura Era ✨</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avm71gmplbwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1cbgrky</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>my hawaii nails</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s34dlf9atawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1cbfpv4</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Did my sisters nails!</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vbxjmrxlawc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1cbe0m4</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Freestyle 3D Gold Chrome. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8w9wmbw9awc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1cbbl1s</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>DUCK DUCK NAILS 🤭</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brhquzhks9wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1cbajvb</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Soft pink set</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbajvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1cb8nyt</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>420 nails babyyyyy</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha86dxrq79wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1cb87r8</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Aura Nails -1st attempt</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yev1a1ao49wc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Apr 25 08:08:21 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_28.xlsx
+++ b/data/2024_04_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C615"/>
+  <dimension ref="A1:C766"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10888,6 +10888,2573 @@
         </is>
       </c>
     </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1ccmepd</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yall... </t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pgh7bvi1lwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1ccmee2</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Got my nails matched to my hair with very a subtle smiley/frown face on my middle fingers 🩷🧡</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuqzmwaf1lwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1ccmczw</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Can it be more nude?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/juhwa0611lwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1cclslz</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Unicorns!! 🦄🦄</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cclslz</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1ccl5o4</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>First time getting almond EVER ✨</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyonsldmmkwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1ccl0wo</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>This sub should be called nailddit</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ccl0wo/this_sub_should_be_called_nailddit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1ccjj1p</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t xml:space="preserve">suggestions? </t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ccjj1p/suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1ccjc02</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Gels lasting a week what am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ccjc02/gels_lasting_a_week_what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1cciums</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Pink nails 🩷</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32q8mc1ixjwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1cchuoc</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>How to do this at home with nail polish</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ytd6ybvnjwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1cchj0b</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Coquette pink nails</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cchj0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1cch77h</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>NAILS!!!</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cch77h</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1ccguhm</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Pink with holo glitter</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccguhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1ccgpjk</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Gel x</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccgpjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1ccgo7g</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Ideas on how to create this effect?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccgo7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1ccgk1l</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Magnet &amp; nuance design</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccgk1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1ccgh5w</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Trying out the blooming gel.</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccgh5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1ccffak</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech ATE! 🤩 These are my natural nails with structured gel! </t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efnbmdee2jwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1ccfatu</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Anime press ons</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ccfatu/anime_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1ccexju</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>I’m a dude who painted his toes for the second time ever! I’m really enjoying this new hobby</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifk5zrt6yiwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1ccexam</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1st time I did powder dip 😀 Does it look okay? </t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tg9iz24yiwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1cce50y</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Haven't had a new set In months! so happy &lt;3 (I promise I will stop biting my cuticles)</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/batw7fk2riwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1ccdsaq</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Am I being too critical or do this look bad?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccdsaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1ccaier</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>🫐🍃🫐🍃🫐🍃</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccaier</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1ccdfk7</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>New Nails, longest they’ve ever been</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/or86q75kliwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1ccd2of</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Petals for the Narcissist</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dh01348oiiwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1cccft5</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>A spring set I had recently. 🐸</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uelqyfomdiwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1ccbbjz</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Here’s my current set !</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccbbjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1ccatmf</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Acrylic Overlay vs Dip</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ccatmf/acrylic_overlay_vs_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1ccam5f</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Anything i can do to fix my nails?</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e92xrdfmzhwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1ccaj2n</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>How to fix lumpy polish</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccaj2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1ccafu7</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Rubber base advise</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ccafu7/rubber_base_advise/</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1cca2em</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Never too old for cat nails.</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmjvoyanvhwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1cc9r63</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Best way to pack gel polish in luggage</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cc9r63/best_way_to_pack_gel_polish_in_luggage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1cc8ptu</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Spring set!! Thoughts on palette and designs?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc8ptu</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1cc8bs7</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starting a job &lt; 1 week </t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cc8bs7/starting_a_job_1_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1cc8ayh</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink frenchies for the win! 🤩 (read caption, I need ideas💡) </t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0w9xd9yihwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1cc8968</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>It was my first time trying this technique so this took over an hour but the end result is DISTRACTING✨</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gpxiykllihwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1cc6syv</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do ya’ll organize your nail supplies? </t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cc6syv/how_do_yall_organize_your_nail_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1cc66nh</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>getting used to short nails again</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc66nh</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1cc32d5</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Press On Application Tips</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cc32d5/press_on_application_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1cc61c4</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Happy with my nails 😍</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axd0inhp2hwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1cc2yai</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>No big toenail... Help?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cc2yai/no_big_toenail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1cc5yf2</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What to ask for and the differences of nail types? </t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cc5yf2/what_to_ask_for_and_the_differences_of_nail_types/</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1cc0jh5</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Olive &amp; June press ons</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cc0jh5/olive_june_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1cbwqfb</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Techs - do you mind clients who don't talk a lot?</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cbwqfb/techs_do_you_mind_clients_who_dont_talk_a_lot/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1cbvcgt</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>I got my nails done for the first time.</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbvcgt</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1cc5h3k</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>DAE have sensory issues with long nails?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cc5h3k/dae_have_sensory_issues_with_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1cc56lh</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Nude with gems set for myself</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc56lh</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1cc54v0</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Builder gel pooling funny on top of Gel X</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/520eouqewgwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1cc5345</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Would you call these round or almond?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qb0u2t42wgwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1cc4tem</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Hand painted tiny picnic nails</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc4tem</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1cc4oif</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>First attempt to semi-permanent! What do you think?</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j94x5cj9tgwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1cc4e84</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>New creation</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc4e84</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1cc39b1</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Lisa Frank it 🦄🌈!</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc39b1</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1cc380u</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>🩵🩵✨</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6p2gdtj7jgwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1cc32rj</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>guysssss i don’t know how to feel 😫</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc32rj</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1cc1ppo</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looove this color ❤️ </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omtk8u1p8gwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1cc19yl</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>🩷✝️💅🏻</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hm2pfdxm5gwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1cc14do</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Clean.</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc14do</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1cc0vcb</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I loved this blue, and the silver rays, it's one of my favorites. </t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsx8q30i2gwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1cbzp3i</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>First MoonCat trial</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sd9gng81ufwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1cbzo9u</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Brand new OPI nail polish not going on smoothly</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbzo9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1cbzhlq</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Red♥️or white🤍team?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbzhlq</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1cbz56j</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Spidey nail art 💅</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9ncdt91qfwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1cbz348</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>SPIDEY NAILS 🕷💅😋</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ggwj33nkpfwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1cbyjpm</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>You like?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbyjpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1cbwnap</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Bunny ears and Easter eggs</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbwnap</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1cbwkkf</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>A little darker but love this red, thought I would go for more of a vampire theme this time, what do you think.</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbwkkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1cbwekm</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Bright color of spring</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpouibmj3fwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1cbw2ht</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>First time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cyc42wog0fwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1cbvgiz</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Less is more! Loving the minimalist vibes on my short nails.</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23s7gp2cuewc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1cbv8ax</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Gold red brown nails</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbv8ax</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1cbtue0</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>General advice</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbtue0</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1cbtcfl</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>nude nails strike again</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e75is0a25ewc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1ccmbre</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>I realize this is completely out of season but I love how cute this combo is</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccmbre</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1ccl19w</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Which products would I use to keep these from getting squished until they grow back in?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1ma1ak7lkwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1ccj7h3</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>I got that dreaded gel allergy...now what?</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ccj7h3/i_got_that_dreaded_gel_allergynow_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1ccij78</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>A true one-coat polish!</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccij78</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1cci8h7</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Do you keep wearing a polish when you don’t like how it looks on you?</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cci8h7</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1cch10f</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>A better look at Quicksand's Embrace done in velvet style</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vsk9xyovfjwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1ccgdl0</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>The chokehold Fairy Dust has me in….</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ek0ckqwjajwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1ccg01s</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Midnight Thunderstorms</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/960f57ld7jwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1ccfzau</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Mooncat magnetic skittle 🦎🦎</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwi2o7p67jwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1ccfgxz</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Harper 😍🧚I keep coming back to this shade</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccfgxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1ccedt1</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>🐝 Mind Your Bees-ness, Honey 🍯</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccedt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1ccdw82</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce Kisses to My X’s</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccdw82</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1ccdr0q</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Golden smog - Death Valley nails</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccdr0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1ccdljq</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Kur Perfecting Veil 1</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9arl0tyxmiwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1ccd7dn</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Glow in the dark</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccd7dn</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1ccd3oz</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Is it… TOO nude?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78ir4itwiiwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1ccd0ra</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>50 Shades of Greige by Holo Taco: unexpected new fave?</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccd0ra</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1ccc2h0</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>First mani pedi-does these look as bad as I think?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccc2h0</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1ccbhbu</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Arctic Monkeys nails ft midly annoyed cat</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3oi1vfd26iwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1ccal41</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>giving Enid a second chance</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccal41</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1ccaec6</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Adventures in magnets</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccaec6</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1ccaa08</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Nail polish based off of these pictures I took?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccaa08</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1cca4vw</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Treachery in the Blue and all its phases</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cca4vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1cca03z</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Ignore my messy stripes and ✨observe the GLOW✨</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cca03z</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1cc9q7d</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Boys, Ugh!</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q584v1h5thwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1cc8mxk</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Since everyone is wearing purple - LA colors, Jazzy</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxjgv9iclhwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1cc8fts</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Wanted to participate in all the thermal rave right now</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkzpz8gxjhwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1cc8eou</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails for Mexico </t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqh5dr3pjhwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1cc828h</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Coffee / Macchiato / Mocha Cloud Dupe?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cc828h/coffee_macchiato_mocha_cloud_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1cc6qir</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>First ever BKL and UP</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc6qir</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1cc6bmg</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Contrary Polish Sparks</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cc6bmg/contrary_polish_sparks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1cc5occ</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>What do you guys think about Brazilian manicures?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pp1b1av40hwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1cc435e</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Are glass foot files worth the hype? 🫣</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cc435e/are_glass_foot_files_worth_the_hype/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1cc41to</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's giving watercolors </t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iz9ervuxogwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1cc3rfr</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>That Went Well.</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc3rfr</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1cc3iyd</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Sally hansen combo</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/whjdk7lblgwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1cc3adl</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Tried something more subtle this week...</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7892tb5ojgwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1cc2pjh</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>When/if to stop using natural nail strengtheners</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cc2pjh/whenif_to_stop_using_natural_nail_strengtheners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1cc28l7</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Tiny flower inspired holo ✨</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc28l7</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1cc23bu</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>blue flower mani after 7 days of wear!</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc23bu</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1cc1ufa</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Daisy, Daisy, Give me your answer, do…</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23u59xfo9gwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1cc1i49</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Dupes for "high fae" by lights lacquer?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc1i49</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1cc1d59</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>It’s giving corpse</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyozi9m86gwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1cc1578</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Recommend a base coat &amp; top coat based on my nail type?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cc1578/recommend_a_base_coat_top_coat_based_on_my_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1cc0g9e</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Help spot the difference</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc0g9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1cc08gg</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Essie Mademoiselle always looks weird on me</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qo9ctbo0yfwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1cbzlv8</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>L' Amour!!</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbzlv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1cbxxvw</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>OPI Repair Mode?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cbxxvw/opi_repair_mode/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1cbxjdu</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Pink marble nails 💖</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbxjdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1cbxfao</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>🏅💜Favorite Blurples💜🏅</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbxfao</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1cbuwqm</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Is this normal for nail salons?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4if8a4ueoewc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1cbwsdg</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>When you live in New Zealand but still want velvetised nails...</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zgq7qvx27fwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1cbvxlg</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Okay but I'm obsesseddddd with my new mani 💖</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbvxlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1cbu4qe</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>My mooncat obsession continues</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbu4qe</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1cbt0p5</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>It’s a closer match in person, I promise</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6i8rb8p0ewc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1ccigxf</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Kuromi press ons 💅🏼</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iy8s9a0wtjwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1cci3fw</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Second try diy press on</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cci3fw</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1cch776</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>TikTok @GetFizzE</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/238y1xgthjwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1ccgpuy</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Unicorns 🦄🦄🦄</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccgpuy</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1ccfpxg</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Chrome Design. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o3jr30uy4jwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1ccfl3b</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Tips, recourses, CC?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccfl3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1ccf4z4</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍒 </t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25uip8uwziwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1ccf3zv</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>I’m in love with this new set. 🤭😍🥰</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jp31pwnnziwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1ccekoe</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Pink Nails</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hn4j8ns2viwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1cccio7</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>What do you think about lipstick nails?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cccio7</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1ccayre</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Little Twin Stars nails ⭐️</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ck6duj92iwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1cc9ynh</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Fun set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5z18dqvuhwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1cc7bcf</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Team🍒 or 🍓?</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc7bcf</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1cc5ez9</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>early 2000s inspired duckies</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hp8d423dygwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1cc4wl2</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Opal Opal 💕</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc4wl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1cc4dn4</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Nails for my 8 year old cousin 💕</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khrugbo5rgwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1cc45di</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When the thumbnail looks awful so you switch up designs halfway through </t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8xkjf5lpgwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1cc26tq</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Cutie spring oranges 🍊 💅🏼</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc26tq</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1cc1lju</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Freestyle set🧜🏾‍♀️🐟</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cc1lju</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1cbv7sq</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried some new designs today. </t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vs2tohvrewc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1cbt1o3</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Well</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cbt1o3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Apr 26 08:08:44 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_28.xlsx
+++ b/data/2024_04_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C766"/>
+  <dimension ref="A1:C907"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13455,6 +13455,2404 @@
         </is>
       </c>
     </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1cdfe1u</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>airbrush slay with gold tips ✨</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdfe1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1cdeve9</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t xml:space="preserve">press ons over gel x </t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cdeve9/press_ons_over_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1cdeeuo</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>I finally got duck nails</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15huwd4qprwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1cddw6s</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t xml:space="preserve">If your hands get red and purple splotched- light blue is your friend! </t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76fqap8yjrwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1cddq8f</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Clean girl✨</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khkfvjq4irwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1cddgom</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Got a beachy look for my upcoming trip to Costa Rica!</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zej6zrbbfrwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1cdcvoe</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>pink spring nails 🌸</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdcvoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1cdc5cp</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>How Bad Do These Look?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dixf3ezw1rwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1cdbovk</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Dashing Diva super gel glue</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cdbovk/dashing_diva_super_gel_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1cdaf9i</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>DND 243 Purply Pink</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e21iqroulqwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1cda6wg</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love these </t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5eeritpjqwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1cd9w8l</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Spring nails: pink with a hint of chrome</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd9w8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1cd9njs</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>classic gel-x french tip</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd9njs</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1cd9cza</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Nail Growth Progress (2 Weeks)</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd9cza</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1cd9cne</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>fluttershy nails</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd9cne</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1cd9bfg</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>My nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lx8f0i1ecqwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1cd8xxg</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>i love these</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd8xxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1cd8tmh</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>First time getting Gel X. Absolutely in love with my new set. Any thoughts on Gel X?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85yr3dm58qwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1cd8ta2</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Made some cat eye and chrome celestial press ons</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ytgnzr28qwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1cd8pu4</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>i'm obsessed with this design! 🌠</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd8pu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1cd8br1</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Wine, anyone? 🍷✨</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd8br1</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1cd7u0b</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Birthday nails 💙🌀🩶🌀</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ixaummszpwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1cd7iut</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>🩷 ILNP Grace ✨ Such an elegant neutral holo!</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd7iut</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1cd6zei</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Vacuum as a Dust collector hack?</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cd6zei/vacuum_as_a_dust_collector_hack/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1cd54au</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>New set 🤍</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd54au</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1cd4uy0</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Girl I like did my nails</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2ykwcl4dpwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1cd4t67</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Fresh and clean</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd4t67</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1cd4kb4</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Stiletto/ oval or square?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd4kb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1cd3ezx</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Simple &amp; Clean</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4qpxzjt1pwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1cd34o0</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>GelX nails I did on myself</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdnlkpguzowc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1cd2kmc</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>I have these gel nail polishes that say they don’t need a UV light but they don’t dry</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vdsdn2eyvowc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1cd2jud</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Hand Painted Nail Art 💖</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd2jud</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1cd2d2e</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Love this color but what is it?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd2d2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1cd21xr</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Can I put polish on this 😒</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnwwm17gsowc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1cd2107</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Did my nail tech eat these lipstick nails?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd2107</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1cd1s00</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Early 2000s vibes</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd1s00</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1cd1q4f</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Is there a good resource for how to get started doing nails?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cd1q4f/is_there_a_good_resource_for_how_to_get_started/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1cd0za5</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Lifting?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd0za5</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1cczwy8</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>my first time, done by myself!</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cczwy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1cczr4t</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Posts/pictures not showing?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cczr4t/postspictures_not_showing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1cczec0</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>What would you add</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94hod31kaowc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1cczbvw</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Tyrone 1mc Nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqnfvfr2aowc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1cczbkl</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>I've found the perfect summery red! 😍</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cczbkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1cczahe</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Purple chrome 🍇🤍</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/giwy30it9owc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1ccz4gf</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>My nails on both hands ended up matching the flowers I came across today!🌺</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccz4gf</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1ccyz2c</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>I love when my vision turns out exactly as I want(set made by me)</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xls16jdo7owc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1ccyt2e</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Shining cute french set ❤</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r03wlg3b6owc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1ccyjfp</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>$55!🤍</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccyjfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1ccyf48</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Does it look alright with having short nails on one hand and long on the other?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ccyf48/does_it_look_alright_with_having_short_nails_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1ccyf11</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>I love how they turned out</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yc7gw8814owc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1ccy1l3</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Can this be accomplished with dip?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xtdwfno1owc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1ccxpf5</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I finally have my nails done and with the color that is in trend, pretty, right?
+</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oizn0p3mznwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1ccxlb4</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Tried a new style, not sure how I feel about it. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7uotbbsvynwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1ccxd3w</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Nail Art🩷🤎💚💜</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulq4x3rgxnwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1ccwzzx</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Love this color but what is it?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccwzzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1ccwigu</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>What do you think of this style? coquette🎀</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ef4tc64vknwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1ccvzc8</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Birthday set</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ig8crs34hnwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1ccvysy</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Claws</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uiuqm9k1hnwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1ccvhz1</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>This color made me feel powerful</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d96n3fttdnwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1ccv66a</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>I finally did them🤭</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccv66a</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1ccuqsd</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Party Glitter 🎉</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9x1oakmf8nwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1ccfhkv</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>I didn't think I'd like pink this much</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccfhkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1cct6ho</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Did this set yesterday and I am in love 😭💕</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lw10fhkywmwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1cct3bk</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>before and after, day 13 of no biting my nails! polished them my favorite color 🩷</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cct3bk</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1cct16e</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Black nails go with everything, don’t they?</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8d9n5z6wvmwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1ccszq1</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Just finished 🥰</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sc9ttm2mvmwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1ccsp74</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Blue butterfly nails 🦋</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d3q7gxaktmwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1ccsiub</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Something different</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tw36ymr8smwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1ccrtb7</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Strawberries!</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccrtb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1ccrcm7</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New color, love it! what do you think? </t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ub47oazvimwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1ccqvbr</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Going to a rodeo on Saturday 🤠</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzq7kaymemwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1ccqtrg</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>In love!</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zuaosk1cemwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1ccqp1e</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Glamrdip</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ccqp1e/glamrdip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1ccon5n</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Growth after one week, do my nails grow super fast? I don’t wanna be stuck redoing my nails every week 🥲 (ignore the bees, nail art is difficult haha) </t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vrzy2lrslwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1ccocxe</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Pink and black, natural nails</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvfbfvbkplwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1ccn59d</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Best budget full-cover tips to make press ons?</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ccn59d/best_budget_fullcover_tips_to_make_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1ccmzro</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>How about blue with white wave?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dw2wtwlq8lwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1ccmlls</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>My new nails~</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zc2vo6yt3lwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1cdepra</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Purple vs violet?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cdepra/purple_vs_violet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1cddcxb</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Come out to socialize</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pdlox2a7erwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1cdcvn9</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Fixed the pink nails</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdcvn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1cdcb3m</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Do you hear the Siren’s song?</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdcb3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1cdc3w2</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do u think for this rose? </t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kpxoboi1rwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1cdbgt0</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Treachery in Blue shift</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vybj717jvqwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1cdawps</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Birthday Girl Layering</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cdawps/birthday_girl_layering/</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1cd9y7v</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Went for a manicure for the 1st time in my life. A no polish manicure. The tech used some kind of sandpaper sponge on my nails. Its been a week, how do I get rid of the scratches? (I'm a nurse. Can't have any product on my nails at work)</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oa0f0zllhqwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1cd9gth</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Question about using nail glue as a base coat</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64k10rcmdqwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1cd9em8</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>How to figure out which polish caused the staining.</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cd9em8/how_to_figure_out_which_polish_caused_the_staining/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1cd8vpg</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Experiences with Girly Bits Glitter Glaze</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmgf2vkn8qwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1cd8sp6</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Sparkling French</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd8sp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1cd8ih1</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Push Play and Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd8ih1</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1cd89dm</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>I’ve been wearing lots of blue lately! 🫐</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd89dm</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1cd7qy2</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>My last mani</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nt8fs6c3zpwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1cd7es4</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>🩷 ILNP Grace ✨ Such an elegant neutral holo!</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd7es4</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1cd5vz3</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Any lord of the rings themed collections or polishes?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cd5vz3/any_lord_of_the_rings_themed_collections_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1cd5bzn</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Birthday Nails &amp; Bee Friend 🐝🌼</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd5bzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1cd4wqq</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Sassy Sauce — Cock-A-Doodle-Doom</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd4wqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1cd4d8h</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Fueling the flames 🔥</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd4d8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1cd4c3z</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Teddy by ILNP 💕</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d0v0sch9pwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1cd465h</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Does anyone else paint the underside of their nails?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd465h</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1cd3xcn</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Pre birthday mani #4...</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y34gsuyi5pwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1cd3eur</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Friend asked me to paint her nails. (Rant)</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cd3eur/friend_asked_me_to_paint_her_nails_rant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1cd37w5</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>New fav</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd37w5</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1cd37mf</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Swamp Gloss- He’s F*ck Ugly</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd37mf</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1cd318z</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Green Goddess (Velvetized)</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd318z</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1cd30ck</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Ethereal arrived gloopy???</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd30ck</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1cd2o7n</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Thanks for turning me onto LynB!</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jfe4oimwowc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1cd2gla</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Painting the underside of the swatch stick did not work for me.</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd2gla</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1cd2axp</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>🏅💜Favorite Purples💜🏅</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd2axp</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1cd1k66</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Finally bought a shifty shimmer…😍</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftpf5op6powc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1cd14bm</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Catch Ya Later Dudes -Polished for Days ✌🏻🌊🏄‍♀️⛅️</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yitu39t6mowc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1ccznlc</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Heather's Hues issues</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ccznlc/heathers_hues_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1ccyk39</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Portable storage for gel nails</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ccyk39/portable_storage_for_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1ccxyo4</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Kraken’s Wrath over a vibrant blue</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccxyo4</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1ccxl0p</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Made a diy blurple!</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bq05fwtynwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1ccxabd</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>GEL Dupe for China Glaze Flame-Bouyant</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ccxabd/gel_dupe_for_china_glaze_flamebouyant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1ccv9ff</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Question on Brands</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ccv9ff/question_on_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1ccuoyq</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Dupe request: Smoky Maple Chai by Potion Polish</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ccuoyq/dupe_request_smoky_maple_chai_by_potion_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1cct0w8</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Cirque Colors “You Tart!”</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cct0w8</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1ccsw29</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Thermal did a thing with cold fingies</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccsw29</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1ccr3p4</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This polish is wild! </t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w6rr814sgmwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1ccr3kc</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Birthday mani 🥳</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccr3kc</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1ccqyie</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OK, that's real pretty </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7izwg6ifmwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1ccpw9x</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Thanks, I hate it</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovp49fis5mwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1cdevl5</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Help! What colour / type of nails should I get to wear with this bridesmaid dress. I am getting BIAB for the first time.</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xsgfpw3vrwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1cddgeo</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Green Cat Eye</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cddgeo</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1cdam92</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Chinese new year themed set!!</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdam92</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1cd8tzs</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Watercolor or nail gels?(done by me)</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ligrmto88qwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1cd4sro</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Nail Art Tutorials</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://youtube.com/watch?v=g4tgBvX7aZg&amp;si=LQVSXctOiL8hPoWC</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1cd40tm</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adding stickers/foil to professionally done acrylics? </t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1cd40tm/adding_stickersfoil_to_professionally_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1cd36d6</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Monochrome Human bones 🦴</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd36d6</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1ccz7ga</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>My first set of press-ons!</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccz7ga</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1cd2mxt</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Love this color combo</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cd2mxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1cd1rx9</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Good vibes ✌🏼☮️🌼</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0ryabpmqowc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1cd19eq</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Best nail art tutorials?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1cd19eq/best_nail_art_tutorials/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1cczrhg</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>press ons by me💋</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c17cir2zcowc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1cczbax</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Spring Set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1rmel2z9owc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1ccyyn5</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>New sets I did for my birthday</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccyyn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1ccvihz</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Hello! New member here. How much does this type of art usually cost in the US?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lysyvimxdnwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1ccp7uj</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>🐙</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ltohrp0zlwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1ccmqwi</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>The press on I made for her, and her feedback photos✨ (by IG: juun.yc)</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ccmqwi</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Apr 27 08:07:55 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_28.xlsx
+++ b/data/2024_04_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C907"/>
+  <dimension ref="A1:C1060"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15853,6 +15853,2607 @@
         </is>
       </c>
     </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1ce7lnu</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Are these ok or am i over reacting?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o327bgwtsywc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1ce7svh</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>I Need To Go To Sleep Cause These Nails Are Getting WEIRD</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce7svh</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1ce3jky</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>how do you feel about this combination of colors?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgs0edycnxwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1ce3977</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Cherry Blossoms 🌸</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce3977</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1ce2vq6</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>ImPress nails</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgf3kg7dhxwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1ce1ygs</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help fitting press ons? </t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9sfkayy8xwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1ce00jj</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Does water damage builder gel and can you use it ad a top coat?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ce00jj/does_water_damage_builder_gel_and_can_you_use_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1cdzn4w</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Cinco de Mayo inspired</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdzn4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1cdybwc</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Can someone explain what I did wrong?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdybwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1cdvqit</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What am I doing wrong???  </t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cdvqit/what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1cdvnqu</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Why do my nails only last with acrylic?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5f5r4kdvvwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1cdvfi2</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Stamp Not Working </t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57krre1ptvwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1cdunii</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why are my nails so fucked up? Can I fix this? </t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbt3iohbovwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1cdlqqt</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>My progress in gel nails.</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdlqqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1cdo9x1</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Help with recommendations! Brooklyn NY</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cdo9x1/help_with_recommendations_brooklyn_ny/</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1cdngvz</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it normal for acrylic nails with gel to be applied only at the tip of your natural nail? Mine fall off because the acrylic is outgrown and no longer supported by the natural nail. </t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cdngvz/is_it_normal_for_acrylic_nails_with_gel_to_be/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1cdn66w</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Soak off acrylics with "ring of fire" drill line?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cdn66w/soak_off_acrylics_with_ring_of_fire_drill_line/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1cdkkto</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Ya girl got proposal-ed</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdkkto</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1cdffn6</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Why do my acrylic nails always point up?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdffn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1ce6j18</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>One hand of my new asymmetrical freestyle set</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tp2cl375hywc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1ce5r5y</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Boyfriend looking for gift advice</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ce5r5y/boyfriend_looking_for_gift_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1ce58hh</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9028df9t3ywc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1ce47jd</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Press on set from Etsy</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rq9rr8omtxwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1ce3qlw</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>purple spring nails 💜</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngfqx749pxwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1ce32is</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UV lamp with regular lacquer? </t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ce32is/uv_lamp_with_regular_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1ce31yw</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blueberries 🫐 </t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blu2c07xixwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1ce2liv</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>First client in months ....</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce2liv</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1ce2jdf</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>I got my nails done today! ☺️</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce2jdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1ce20ul</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Nail color regret 😭</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdt43dbl9xwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1ce1yoa</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>My nails and tiny tattoo from valentines day</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce1yoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1ce1sfc</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Cutsy vampy nails</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce1sfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1ce1s5a</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>in love with this set</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce1s5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1ce1r7d</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Had some fun with these colors!</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jevfik87xwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1ce19hf</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Accidentally matched my nails to like... Half the stuff I own lol</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce19hf</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1ce17el</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Trying a different nail shape  - NO!</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ce17el/trying_a_different_nail_shape_no/</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1ce152k</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second time attempting a “Gel X” set at home, be gentle </t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1dbh8bru1xwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1ce0qfn</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>How to strengthen nails?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ce0qfn/how_to_strengthen_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1ce0ehm</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Spring flowers 💙</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbu0lnusvwwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1ce0bm6</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>First time doing gel tips</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce0bm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1ce07ro</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>A little grown out but this mani saw Mariah Carey last weekend</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fgqq4j89uwwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1ce04f1</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Should I try and get acrylics or try and grow my natural nails?</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ce04f1/should_i_try_and_get_acrylics_or_try_and_grow_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1cdzxzo</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Nail growth journey!</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdzxzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1cdzf9u</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Decided to go with light pink after red design🤍</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdzf9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1cdyvlt</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>My nails :) freshly done</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gp0q95xgjwwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1cdygan</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Tried out spider gel for first time</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r59z6ik3gwwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1cdxzqq</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Sally Hansen Xtream Wear Polish</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdxzqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1cdxreo</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>A bit of a red fever😍♥️🌹🍷</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdxreo</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1cdx8b4</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Who else allows their nails to grow out a fair bit before an infill to make the infill seem worthwhile?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9toke2w6wwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1cdx18g</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Aura nails</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d053otdf5wwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1cdwx81</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Obsessed with this color</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdwx81</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1cdwtjm</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Lavender tips anyone ? 💜</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdwtjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1cdwdqt</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Kiss Impress</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdwdqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1cdvz0h</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>What's the best way to measure your nails?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cdvz0h/whats_the_best_way_to_measure_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1cdvkx6</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Do these look okay?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ot2jwm7suvwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1cdvbs0</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>{PR} Dragon Nail Art</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdvbs0</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1cduije</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Newbies 🧡🧡</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cduije</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1cdtwyf</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Childhood me is screaming with glee 🥰🥰</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdtwyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1cdtevy</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>What do you prefer? Long or short?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdtevy</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1cdt7vu</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>spring vibes &lt;3</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2a0e5popdvwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1cdstdp</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Guess how many polishes I used and how many hours these nails took me 👀</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdstdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1cdss7g</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Got my biab nails infilled and a cats eye mani for my night out tomorrow 🖤🤍</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0bad8xgavwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1cds0si</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just driving around </t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e62dxi8z4vwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1cdrxie</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Please tell me there is a way to protect this until it heals?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cdrxie/please_tell_me_there_is_a_way_to_protect_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1cdrp79</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Really like how these turned out!!</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdrp79</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1cdrlq4</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Acrylics aren’t in my budget right now so thought I’d try Kiss press ons. Is it typical for their clear nails to turn pink??</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arc3m1aw1vwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1cdqyl2</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>✨️✨️✨️</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yyr1qt08xuwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1cdq78k</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Do you like bright sun shine?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yvt88h8lruwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1cdq6rn</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>dip, gel x, or acrylic</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqk2p4tlruwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1cdq4x6</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Holo glitter square nails</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdq4x6</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1cdq402</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Newbie Gel-X chrome French ombre</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwzn23q1ruwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1cdpzw7</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Tomorrow is Kingsday in The Netherlands 👑🇳🇱 I’m a teacher &amp; kids every age loved it. Some even tried to remake it on their nails 😁 (2 weeks old set btw)</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aubh4rh8quwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1cdpqaq</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>How can I prevent this yellowing on my nails?</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5gd5etaouwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1cdop1y</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>What nails would go with this dress?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2aszhsvguwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1cdnult</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>amethyst crystal with gold</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdnult</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1cdmrsv</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Do you think it’s time for a new set?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4q22mf2t2uwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1cdmmyk</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Acrylic gel paint has cracked - can I just use normal nail polish to paint over it for the meantime till my next infill?</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1eanc2vt1uwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1cdmbeo</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>My First Set Ever Made And First Time Doing Nails</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojbk3g9hztwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1cdm5wx</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Do you hear the Sirens song?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdm5wx</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1cdhw0w</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Pink builder gel with glitter fade 💗</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gy87720wswc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1cdh6zt</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2000s style gel nail set </t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cdh6zt/2000s_style_gel_nail_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1cdfz3o</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Another goid nail day</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdfz3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1cdcgw2</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best cheap nail supplies/polish? </t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cdcgw2/best_cheap_nail_suppliespolish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1cd9vwj</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Went for a manicure for the 1st time in my life. A no polish manicure. The tech used some kind of sandpaper sponge on my nails. Its been a week, how do I get rid of the scratches? (I'm a nurse. Can't have any product on my nails at work)</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0yr4gix2hqwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1cd9bxg</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>nintendo vibes</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pz7tbyficqwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1ce6nhv</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>ILNP Fairy Dust…I’m in love</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0nhwjfiiywc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1ce62ip</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Polish changing at altitude?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ce62ip/polish_changing_at_altitude/</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1ce60o1</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Show me your favorite ILNP polish!</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ce60o1/show_me_your_favorite_ilnp_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1ce5sec</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Moonicorn</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce5sec</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1ce4ncf</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Starrily Magma over Cirque Indigo Jelly</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cea1ey9wxxwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1ce3eef</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>[Static Nails] Coconut</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93d15963mxwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1ce3y3y</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Help fitting press on nails?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce3y3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1ce2x97</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>ILNP's Jet Setter is so mesmerizing 😍💜</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upqqfworhxwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1ce2c8h</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Nail polish &amp; raccoons</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce2c8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1ce1bp0</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me find this Redditor! </t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ce1bp0/help_me_find_this_redditor/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1ce18ah</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Help with OPI shade ID!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce18ah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1ce1822</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Minimalist Abstract Polka Dots ~ Yay or Nay?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce1822</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1ce05hv</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>💙I love blues</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce05hv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1ce04tn</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>“How Can These Legendary Hands Help You?” 🤯</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36827m2ktwwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1ce04or</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Took these to see Mariah Carey last weekend </t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/moxsuidktwwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1cdzslf</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>I can’t get over how beautiful and shifty these look!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/11blapcqqwwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1cdzl9m</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>A lil matchy moment</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdzl9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1cdz9m4</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>This shade is just so magical 🤩💜</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pja5nealmwwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1cdxy4w</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Queen of Rot- Bee's Knees Lacquer</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmfmwsw0cwwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1cdsa9q</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>I can't get over 'Am I Everything You Fear?' from Mooncat's new collection 👌</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpmr0skg6vwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1cds6ze</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>This is your sign to try Mooncat's 'Foxfire' over 'Am I everything you fear?'</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dh78v826vwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1cdxl5q</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Mooncat polish</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdxl5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1cdvrbj</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Sugar Daddy</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdvrbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1cdvmgl</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Someone spilled paint in the back of my work truck while I was off yesterday and the paint happened to match my nails </t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58qg77r3vvwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1cduwon</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Need advice/opinions pls 🙏</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cduwon</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1cdur58</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Glowy 🩵💙💜</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdur58</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1cduib7</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Raindrops ☔️</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cduib7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1cdueqq</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Rainbow skittle, but make it *spring*</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdueqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1cducfs</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>💖✨️ Glowy Skittle!! ✨️💖</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cducfs/glowy_skittle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1cdu0ad</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Help identifying color</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxsba56hjvwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1cdtdtg</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Love the addition to my green collection!</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdtdtg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1cdt14e</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Bottle vs Swatched</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdt14e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1cdsx6q</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Lilac Inspired Amalgamation</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdsx6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1cdsuld</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Dino Nails 🦖</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdsuld</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1cds6jy</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Life in plastic vs Pinkies up</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cds6jy/life_in_plastic_vs_pinkies_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1cds3q9</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>i love this color combo</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pb4mwddj5vwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1cdqzqs</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The holo is holoing </t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dpvmcmgxuwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1cdqzei</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>✨️✨️✨️</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/natrmo8exuwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1cdqmwt</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Holo Taco Retro Collection Rainbow</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdqmwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1cdqdv2</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Nail art kit</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ha056l0tuwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1cdq5pk</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Holo glitter square nails</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdq5pk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1cdpwdk</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>One of my favorites polishes in my collection</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdpwdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1cdpqmq</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sally Hansen 540 frutti petutie </t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cdpqmq/sally_hansen_540_frutti_petutie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1cdpjvc</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>🏅💖Favorite Fuchsia💖🏅</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdpjvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1cdpik7</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>I haven't mastered magnets yet but I'm still happy</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/my7go84smuwc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1cdph72</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why does my acrylic nail break like this? </t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhsvd2gimuwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1cdpbu7</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>💖🍬💖</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdpbu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1cdp2vf</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shifty 🐍 nails! </t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/85en237pjuwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1cdov66</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Confetti First Timer</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdov66</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1cdogaa</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Color Club Ocean Spray</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdogaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1cdnsti</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>The Moonstone Shade of my Dreams</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdnsti</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1cdnp2f</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Juicy fruity nails</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdnp2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1cdn5du</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Too many purples…</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3z9unhnm5uwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1cdmvyc</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Diamond mani</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdmvyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1cdmji4</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Loving my nails!</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdmji4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1cd68z2</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>What undertones do I have and what colors would look best on me?</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o870ldicnpwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1cdhwxk</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Please help me find a shade of polish like this (preferably a drugstore brand)</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdhwxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1cdkqbi</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>BIAB lifting when growing out</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cdkqbi/biab_lifting_when_growing_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1cdj04p</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jelly Skittles 💅 </t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06e76ywn7twc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1cdhulc</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Mom always had Revlon polish growing up. Used a CVS coupon to pick one up for free. I like it!</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvud6hjlvswc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1ce62wq</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Cherry Blossoms 🌸</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce62wq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1ce5m5s</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Trying to level it up but im still mediocre 😥😥😥</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce5m5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1cdx16v</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>golden hour ☀️</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdx16v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1cdwau9</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>My Second Ever Nail Creation I’ve Done</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kz8tvlo20wwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1cduo0f</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Longest set I’ve ever worked on!! Guess how many polishes I used</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cduo0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1cduivq</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Go bold or go home 🍒</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cduivq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1cduf69</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>I love using video games for color palettes of nail sets!! Nightmare Zero from Megaman X6 inspired nails!! 💜🖤💚</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmh2iv0lmvwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1cdq3xo</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Holo glitter square nails</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cdq3xo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1cdok2j</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fun short set. IG@NailsbyTim6 </t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6whdu2nwfuwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Apr 28 08:08:30 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_28.xlsx
+++ b/data/2024_04_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1060"/>
+  <dimension ref="A1:C1203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18454,6 +18454,2437 @@
         </is>
       </c>
     </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1cf06l4</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Back to the basics</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cf06l4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1cf03x6</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Nail bent.</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cf03x6/nail_bent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1cez72u</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Press on nail glue mess</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cez72u/press_on_nail_glue_mess/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1ceyk4m</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Cat eye effect 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cn0vol3gm5xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1ceyize</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>I’m in love with my new rainbow chrome press on nails</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceyize</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1ceyfy9</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>My Nail Artist @PioPioNails always making my nails amazing 💅🏻 handmade charms &amp; hand painted anime characters 🥹</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceyfy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1ceyb25</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceyb25</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1cey1jl</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>A week of wear and tear on Holo Taco’s “The Floor Is Guava</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5v4bixpg5xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1cexxjv</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Builder gel with gold glitter gel polish on top</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/me3e1nlgf5xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1cexj6j</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Long nailed girlies - how to switch out jewelry?!</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cexj6j/long_nailed_girlies_how_to_switch_out_jewelry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1cex032</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Not sure how i feel about this settt</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cex032</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1cevxgz</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fiji Airbrush Nails </t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pqsdm41v4xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1cevs06</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Froggy press ons! </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86divxqjt4xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1cev0fb</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Glue gets dirty</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cev0fb/glue_gets_dirty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1ceuwv3</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>First time with bio gel 💅</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceuwv3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1ceuhhp</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Aussies, where do you get your supplies?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ceuhhp/aussies_where_do_you_get_your_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1ceu5xg</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>nails for may 🌱🖤</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceu5xg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1ceu1vo</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>I made mistakes, but overall I'm happy with the result :)</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yln767y4d4xc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1cetm9g</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>New set - Been feeling the chrome lately 💕</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/028811h494xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1cetab8</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>🤍</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cetab8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1cet9b4</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>🍒 Red</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cet9b4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1cet1j3</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>A dad on a mission - reverse. She wanted to do my nails, she even wore my magnifying headlamp.</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cet1j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1cesnpw</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>😐</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8y1jblky04xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1cesl0f</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Keeping it short for work</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fipfupsb04xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1ces39c</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>My birthday nails from September ❤️</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8910zxq6w3xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1cerv3i</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>🍊💜</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cerv3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1cerpgu</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Nude almond 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/67q4ey21t3xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1cerkgc</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Koi fish nails 🪷 🌊 </t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2kmf6dxur3xc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1cerhk9</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>2000s style pedicure update</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cerhk9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1cer7ri</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2eu33hyo3xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1cer40o</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>First time doing a design by hand</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x77691c5o3xc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1ceqgtr</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Beginner here. What do you think? First time I built with gel.</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fe0wf6izi3xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1ceq2sd</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Bday nails :3</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ah89b1yxf3xc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1cepqxg</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>My fresh nails</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqac43nad3xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1cep0b2</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Nail techs can “smell everything” when they take your nails off?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cep0b2/nail_techs_can_smell_everything_when_they_take/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1ceopj3</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>What are the nail masks called?</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ceopj3/what_are_the_nail_masks_called/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1cenxr8</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Should I book under UV gel or acrylic for these?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cenxr8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1cens6b</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Fickle!</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cens6b/fickle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1cenepl</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with these </t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4zmkab1v2xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1cenaej</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Any gamers in r/nails? 👀✨🦋</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9tiagz4u2xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1cen6u5</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Vampire fangs 🧛 🦇 🩸</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cen6u5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1cen2gz</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Mooncat x Nightmare Before Christmas glow in the dark polish in Ragdoll (bonus dark pic)</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cen2gz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1cemvyx</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cemvyx/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1cemuw2</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>thick cuticles</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cemuw2/thick_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1cemodl</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple and black ombre with a blacked out nail. </t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8w6iqg2cp2xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1cemhny</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Would square or short ballerina shape look good with my hand/fingers?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cemhny</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1celp9i</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>How did they do?</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1celp9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1celod3</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Ugliest toes</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrcjon5nh2xc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1cekw9v</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>BKL Queen of Rot in the mega bright light of my ice rink 👑⛸️</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kd82lvvnb2xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1cekqd5</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DYI acrylics with pink gems 🩷 </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tw1mxrmia2xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1cekm5a</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>New nails who this</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cekm5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1cek9un</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Holy forking shirt balls, that’s shifty</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kmdsoj4572xc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1cejxi8</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>2nd time trying a gel x set. How did I do?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dtlbdvj42xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1cejfua</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>DIY marble nails with pearl accents</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cejfua</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1cejbkk</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Jelly Strawberries for Spring 🍓</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cejbkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1cej80k</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Not a fan of my nails short, but they got a much needed trim 🍒🍒</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bchojry2z1xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1cej3ys</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>🩷</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avsi4ez7y1xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1ceiu2r</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Guy here. Not the best I’ve done. What do you think?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceiu2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1ceiem7</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Progress from 10/23 to 04/24</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceiem7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1cei8rn</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Lately I've been loving glitter polishes too much ✨</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bi0w3ngr1xc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1cei7jc</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shade: Tribal sun 🌞 </t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jq68c0z7r1xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1cehawu</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Glitter nail dip</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glz890a8k1xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ceh3ld</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>can anyone recommend a glass nail file or any other must have nail care items for natural nails?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ceh3ld/can_anyone_recommend_a_glass_nail_file_or_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1ceh7kh</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Spring Flowers 💙✨</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4f4cz1yhj1xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1ceexsz</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inspired by the Weather &amp; My Mood Recently </t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6n45b9111xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1cec8zl</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>I got my nails done and they lasted a day</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cec8zl/i_got_my_nails_done_and_they_lasted_a_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1ceh5nq</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>❤️</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tb0yguq2j1xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1cefgdw</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Would you be happy with this?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cefgdw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1cee8tz</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Shout out to Aster boy for helping me model my vacation nails</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cee8tz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1cee2rh</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>🍓❤️🍓</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xu3l7h5ct0xc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1cedll2</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Press ons and Dip powder🫣</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cedll2/press_ons_and_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1cedhbg</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Star Wars Day!</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dg319jvtn0xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1cedayz</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Haven’t had my nails done in over a year 🤍🖤🐼 Found the perfect backdrop to show them off</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cedayz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1cebc9l</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>7 DIY later…</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cebc9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1ceb37j</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>This month’s set</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgyw32y4yzwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1ceapo4</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Just finished painting Billie eilish's iconic green phase on some press ons ☺️💚</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2cojbp3ltzwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1ceagim</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Which Nail Shape and Size would Suit me the best??</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceagim</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1ce9gzi</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Did my sisters birthday nails 🌼🌸</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce9gzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1ce9cda</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Summer ready🍊</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce9cda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1cf0td4</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>What nail polish is this?</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cf0td4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1cey03d</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>A week of wear and tear on Holo Taco’s “The Floor Is Guava”</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9puew0f9g5xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1cexydk</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>🌵🌄 🏜️ I was consumed by the urge to reverse stamp and I'm glad I leaned into it (contains PR)</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cexydk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1cewzvo</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Finally did a skittle mani 😍</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ysy37om55xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1cewol5</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>bf thinks nail polish is $6 and who am i to correct him?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cewol5/bf_thinks_nail_polish_is_6_and_who_am_i_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1cevnrr</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>First skittles attempt</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s19auumes4xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1ceuxmu</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>This is one of my all time favourites 😍✨️</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srjudz3el4xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1cety2b</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>🏅🩷Fave Pinks🩷🏅</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cety2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1cesro9</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Y'all sold me on ILNP</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7un2xrhw14xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1ces39x</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>One coat white recommendations?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ces39x/one_coat_white_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1cervql</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Pahlish Lolly</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzcqygihu3xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1cerunv</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is there anywhere to donate nail polish? </t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cerunv/is_there_anywhere_to_donate_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1cerjrp</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Soggy spring day = froggy nails!!</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cerjrp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1cerb14</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Swatch request: Clionadh Squiggles and Mooncat Mermaid Bait</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6h6b98qp3xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1ceqg95</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>⭐️ "Star Fragments" - Polished For Days ⭐️</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceqg95</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1cepzx4</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Puppy Kisses</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyxdrc4bf3xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1cepuig</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Stamping Plate with Tools?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cepuig/stamping_plate_with_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1cepsur</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>LynB - Grey-t Expectations</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cepsur</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1cep91y</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>not sure I like this on me, but I LOVE the way my tips look in the light</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cep91y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1ceop2k</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Ethereal Careful I Bite is so pretty it almost brought me to tears</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceop2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1ceofo2</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Scarlet to violet skittle</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceofo2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1ceo18s</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Waka Waka!</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ceo18s/waka_waka/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1cemtc8</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Last Year’s Halloween Nails 👻</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cemtc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1cemmn5</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone else prefer shorties for spring and summer? </t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2201wo7zo2xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1cemmj7</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Is this what ombre should look like?</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axk2jbixo2xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1cem80u</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce PPU A pain in the asteroid</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cem80u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1celaxm</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>How many back to back gel manicures is it safe to get?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1celaxm/how_many_back_to_back_gel_manicures_is_it_safe_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1cel3ss</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Different but the same, and one that’s plain</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cel3ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1cektg3</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>BKL Queen of Rot in the mega bright light of my ice rink 👑⛸️</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5i9ewaya2xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1cek6qj</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>It’s a party on my nails! 🎉</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tdhcsmh62xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1cejaf6</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Passenger princess admires her nails</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cejaf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1cej79g</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Polished for days -- shadow on the moon</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cej79g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1cej360</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>White tips of nails always very visible through sheer/jelly nail polish, any way to fix this?</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cej360</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1ceirzg</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Matcha + Tencha</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceirzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1ceih7q</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>New favourite nude polish!!</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3g24p808t1xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1cegw66</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>achromatic springtime nails</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/quxpnhs0h1xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1cegryg</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>not a great way to start the day😭</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cegryg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1cegj64</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Springtime glitter ✨</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cegj64</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1cef4l7</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>LynB Simply Iris-istable</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cef4l7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1ceeq4d</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Super Juiced</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1r3llum4z0xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1ceeha3</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Phoenix Indie Polish - Ivy 🌿</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceeha3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1cee5zz</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So many Glass Frog dupes and near-dupes lately. </t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z8yy3mt4u0xc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1cedxi6</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Cirque Morningtide x DVN Cornflowers is a pastel dream~</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wk3lq42s0xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1ced1bc</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>How to get this pearl-like effect?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5uxdsmdfj0xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1cebvxf</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>I love this collection!</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m864cqk570xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1ce66xp</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Yay lesbian nails!</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ce66xp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1ceajk8</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Crome</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3y6dv5kgrzwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1cea08x</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Koningsdag nails!</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxqn2qn4lzwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1ce9s6y</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Cirque Colors Mystic Moonstone 🌙✨</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjc708mbizwc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1cf0roe</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Colorful spring set</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hbub7vwb6xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1cezs3i</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Press-on nail set for my bestie✨ Inspired by To the hellfire a song by Lorna Shore🔥🦇</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nsk3kajd06xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1ceyna9</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>rangi ya vuli🍂</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gedlioen5xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1cev4gn</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Tested my creativity, rate it 1-10🦋</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4awf1k6n4xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1ceu4xs</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>I made mistakes, but overall I'm happy with the result :)</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zeysrswd4xc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1cety5h</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Squiggles and Starbursts </t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pc3s4ge5c4xc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1cesaoe</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>First time doing almond nails😊</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d73o67fxx3xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1ceq5as</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>First attempt at gel nail art</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1eay0nhg3xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1cep18l</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jamaican flag nail art (I tried) 🇯🇲 </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/figy1fpl73xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1cenz90</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>kisses on nails for my client 💋💋💋</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cenz90</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1celi5y</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Similar to my last set</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r37tkwzbg2xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1cehanu</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Butterfly nails for the win</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cehanu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1ceebce</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>I made a new press on set</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ceebce</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1cee8pr</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Do you find such tutorials helpful?</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ht97zk0tu0xc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1ceaq87</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Just finished painting Billie eilish's iconic green phase on some press ons ☺️💚</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d0agbysrtzwc1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>